<commit_message>
0 at deadband. max can be <1. Shape forward too.
</commit_message>
<xml_diff>
--- a/documents/ShapeTurn.xlsx
+++ b/documents/ShapeTurn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3762cd303e452cea/Documents/Robotics2021/2021-Falcon/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{00258F6B-5F49-4C88-8296-7C9BDB565E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE7614AB-4EC9-4713-A216-96ABA37EE035}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="8_{00258F6B-5F49-4C88-8296-7C9BDB565E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{941C1BB1-265A-4A60-940A-D31E9F9115C7}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" activeTab="1" xr2:uid="{768FAE63-1FE3-4B9A-9395-A3569413DFEF}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Input</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Offset</t>
   </si>
   <si>
-    <t>Now plot resulting regression equations to insert into code</t>
-  </si>
-  <si>
     <t>I set this below the 0.15 deadband, so that it will still get driven to zero.</t>
   </si>
   <si>
@@ -91,12 +88,15 @@
   <si>
     <t>exp</t>
   </si>
+  <si>
+    <t>max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +112,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,12 +136,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -186,45 +212,24 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
-      </bottom>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -240,7 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -249,10 +253,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2522,37 +2527,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19263804112167671</c:v>
+                  <c:v>0.20202597087607579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2209980332918598</c:v>
+                  <c:v>0.23005619569544281</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25081207335382372</c:v>
+                  <c:v>0.2595235608729653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.31510432196398808</c:v>
+                  <c:v>0.32306822519696493</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38615824538563109</c:v>
+                  <c:v>0.39329594020672842</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46468497516640517</c:v>
+                  <c:v>0.47090956847842369</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.55147043321170142</c:v>
+                  <c:v>0.55668589329063511</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.64738319755523721</c:v>
+                  <c:v>0.6514833929325019</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75338319537995602</c:v>
+                  <c:v>0.75625083264297976</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.87053131029191688</c:v>
+                  <c:v>0.87203676017224341</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
@@ -2645,37 +2650,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14789148953293979</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15319116737981864</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15966420851935689</c:v>
+                  <c:v>7.6440406502485993E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17722704146168422</c:v>
+                  <c:v>2.8384061615765351E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20342770940559585</c:v>
+                  <c:v>5.9324537121721005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24251451293902115</c:v>
+                  <c:v>0.10548230263827044</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.30082517180203705</c:v>
+                  <c:v>0.17434159722379344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.38781445282961913</c:v>
+                  <c:v>0.27706759354863236</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51758721069662317</c:v>
+                  <c:v>0.4303167719558339</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.71118541596364016</c:v>
+                  <c:v>0.65893768119692997</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
@@ -3018,778 +3023,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Regressions</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Shape w offset'!$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Input</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Shape w offset'!$A$27:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Shape w offset'!$A$27:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4772-4F5B-ABB5-88F8EDBD0F21}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Shape w offset'!$B$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>exp1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Shape w offset'!$A$27:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Shape w offset'!$B$27:$B$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.14000837931780008</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.19262514867268199</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.22099013408614587</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25081221724361547</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.31511695886641533</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.38616992155255503</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.46468482748916695</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.55145857303904222</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.64737122874063091</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.75338603930804171</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.87054942363104204</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.99999097477505849</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4772-4F5B-ABB5-88F8EDBD0F21}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Shape w offset'!$C$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>exp4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Shape w offset'!$A$27:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Shape w offset'!$C$27:$C$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.14134691292508222</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.14593599611065727</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15187994751269807</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.15953280649103985</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.17915649329318784</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.20546178709383356</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.24273899981948358</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.29891402474641893</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.38554833650069487</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.51783899105814157</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.71461862574436208</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.99835545923473523</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4772-4F5B-ABB5-88F8EDBD0F21}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Shape w offset'!$D$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>manual</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Shape w offset'!$A$27:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Shape w offset'!$D$27:$D$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.622299602736299E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.0061981147694356E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.11434986428587388</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.13106657169256461</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1561847066949581</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.18962597977074175</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.24826094269403809</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.34162110539722546</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.47189893597093802</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.63394786066406683</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.81528226388375635</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.99607748819540898</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-4772-4F5B-ABB5-88F8EDBD0F21}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="454748808"/>
-        <c:axId val="454744544"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="454748808"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="454744544"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="454744544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="454748808"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="0.1"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3910,46 +3143,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4983,522 +4176,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6098,13 +4775,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>405493</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>97971</xdr:rowOff>
+      <xdr:rowOff>97970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>250373</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>103413</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6126,44 +4803,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>166006</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>130629</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>321129</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>48987</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA31FDD4-B885-4605-9096-5E21BB40E6C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6471,7 +5110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4E0B77-4DB4-4B7B-A44F-9580F4BD9F83}">
   <dimension ref="A2:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -7304,10 +5943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8CB8AF-B239-41A9-A214-B9F0B9D430C1}">
-  <dimension ref="A2:F38"/>
+  <dimension ref="A2:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -7316,537 +5955,253 @@
     <col min="5" max="5" width="12.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="D3" s="7" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8">
-        <v>0.14000000000000001</v>
+      <c r="E3" s="7">
+        <v>0.15</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="str">
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11" t="str">
         <f>CONCATENATE(F5,F6)</f>
         <v>exp4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A6" s="10">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9">
+        <f>(EXP(A6)-1)/(EXP(1)-1)*(1-$E$3)+$E$3</f>
+        <v>0.15</v>
+      </c>
+      <c r="C6" s="12">
+        <f>(POWER(EXP(IF(A6&lt;E$3,0,A6-E$3)),F$6)-1)/(POWER(EXP(1-E$3),F$6)-1)*F$9</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <f>EXP(0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="9">
+        <f t="shared" ref="B7:B17" si="0">(EXP(A7)-1)/(EXP(1)-1)*(1-$E$3)+$E$3</f>
+        <v>0.20202597087607579</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" ref="C7:C17" si="1">(POWER(EXP(IF(A7&lt;E$3,0,A7-E$3)),F$6)-1)/(POWER(EXP(1-E$3),F$6)-1)*F$9</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="M7">
+        <f>EXP(1)</f>
+        <v>2.7182818284590451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="B8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.23005619569544281</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <f>(EXP(A6)-1)/(EXP(1)-1)*(1-$E$3)+$E$3</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ref="C6:C17" si="0">(POWER(EXP(A6),F$6)-1)/(POWER(EXP(1),F$6)-1)*(1-$E$3)+$E$3</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>0.1</v>
-      </c>
-      <c r="B7">
-        <f t="shared" ref="B7:B17" si="1">(EXP(A7)-1)/(EXP(1)-1)*(1-$E$3)+$E$3</f>
-        <v>0.19263804112167671</v>
-      </c>
-      <c r="C7">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B9" s="9">
         <f t="shared" si="0"/>
-        <v>0.14789148953293979</v>
-      </c>
-      <c r="D7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>0.15</v>
-      </c>
-      <c r="B8">
+        <v>0.2595235608729653</v>
+      </c>
+      <c r="C9" s="12">
         <f t="shared" si="1"/>
-        <v>0.2209980332918598</v>
-      </c>
-      <c r="C8">
+        <v>7.6440406502485993E-3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="B10" s="9">
         <f t="shared" si="0"/>
-        <v>0.15319116737981864</v>
-      </c>
-      <c r="D8">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9">
+        <v>0.32306822519696493</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" si="1"/>
+        <v>2.8384061615765351E-2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.39329594020672842</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="1"/>
+        <v>5.9324537121721005E-2</v>
+      </c>
+      <c r="D11" s="8">
         <v>0.2</v>
       </c>
-      <c r="B9">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="B12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.47090956847842369</v>
+      </c>
+      <c r="C12" s="12">
         <f t="shared" si="1"/>
-        <v>0.25081207335382372</v>
-      </c>
-      <c r="C9">
+        <v>0.10548230263827044</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="B13" s="9">
         <f t="shared" si="0"/>
-        <v>0.15966420851935689</v>
-      </c>
-      <c r="D9">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>0.3</v>
-      </c>
-      <c r="B10">
+        <v>0.55668589329063511</v>
+      </c>
+      <c r="C13" s="12">
         <f t="shared" si="1"/>
-        <v>0.31510432196398808</v>
-      </c>
-      <c r="C10">
+        <v>0.17434159722379344</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="B14" s="9">
         <f t="shared" si="0"/>
-        <v>0.17722704146168422</v>
-      </c>
-      <c r="D10">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>0.4</v>
-      </c>
-      <c r="B11">
+        <v>0.6514833929325019</v>
+      </c>
+      <c r="C14" s="12">
         <f t="shared" si="1"/>
-        <v>0.38615824538563109</v>
-      </c>
-      <c r="C11">
+        <v>0.27706759354863236</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="B15" s="9">
         <f t="shared" si="0"/>
-        <v>0.20342770940559585</v>
-      </c>
-      <c r="D11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>0.5</v>
-      </c>
-      <c r="B12">
+        <v>0.75625083264297976</v>
+      </c>
+      <c r="C15" s="12">
         <f t="shared" si="1"/>
-        <v>0.46468497516640517</v>
-      </c>
-      <c r="C12">
+        <v>0.4303167719558339</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="B16" s="9">
         <f t="shared" si="0"/>
-        <v>0.24251451293902115</v>
-      </c>
-      <c r="D12">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>0.6</v>
-      </c>
-      <c r="B13">
+        <v>0.87203676017224341</v>
+      </c>
+      <c r="C16" s="12">
         <f t="shared" si="1"/>
-        <v>0.55147043321170142</v>
-      </c>
-      <c r="C13">
+        <v>0.65893768119692997</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="10">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
         <f t="shared" si="0"/>
-        <v>0.30082517180203705</v>
-      </c>
-      <c r="D13">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>0.7</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="1"/>
-        <v>0.64738319755523721</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.38781445282961913</v>
-      </c>
-      <c r="D14">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>0.8</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="1"/>
-        <v>0.75338319537995602</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0.51758721069662317</v>
-      </c>
-      <c r="D15">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>0.9</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="1"/>
-        <v>0.87053131029191688</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0.71118541596364016</v>
-      </c>
-      <c r="D16">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17">
+      <c r="C17" s="12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
+      <c r="D17" s="8">
         <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" cm="1">
-        <f t="array" ref="A20:E20">LINEST(B$6:B$17,A$6:A$17^{1,2,3,4})</f>
-        <v>3.4655906524502657E-2</v>
-      </c>
-      <c r="B20">
-        <v>7.0435428721087531E-2</v>
-      </c>
-      <c r="C20">
-        <v>0.25495841872953834</v>
-      </c>
-      <c r="D20">
-        <v>0.49993284148212985</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0.14000837931780008</v>
-      </c>
-      <c r="F20" t="str">
-        <f>B5</f>
-        <v>exp1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="9" cm="1">
-        <f t="array" ref="A21:E21">LINEST(C$6:C$17,A$6:A$17^{1,2,3,4})</f>
-        <v>1.514825562405979</v>
-      </c>
-      <c r="B21" s="10">
-        <v>-1.4057037996172661</v>
-      </c>
-      <c r="C21" s="10">
-        <v>0.76605971025713671</v>
-      </c>
-      <c r="D21" s="10">
-        <v>-1.8172926736196488E-2</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0.14134691292508222</v>
-      </c>
-      <c r="F21" s="12" t="str">
-        <f>C5</f>
-        <v>exp4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22" cm="1">
-        <f t="array" ref="A22:E22">LINEST(D$6:D$17,A$6:A$17^{1,2,3,4})</f>
-        <v>-3.0579341007267513</v>
-      </c>
-      <c r="B22">
-        <v>7.0928663700378909</v>
-      </c>
-      <c r="C22">
-        <v>-4.2855590739648841</v>
-      </c>
-      <c r="D22">
-        <v>1.2450819932464168</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1.622299602736299E-3</v>
-      </c>
-      <c r="F22" t="str">
-        <f>D5</f>
-        <v>manual</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="str">
-        <f>B5</f>
-        <v>exp1</v>
-      </c>
-      <c r="C26" t="str">
-        <f>C5</f>
-        <v>exp4</v>
-      </c>
-      <c r="D26" t="str">
-        <f>D5</f>
-        <v>manual</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <f>A$20*A27^4+B$20*A27^3+C$20*A27^2+D$20*A27+E$20</f>
-        <v>0.14000837931780008</v>
-      </c>
-      <c r="C27">
-        <f>A$21*A27^4+B$21*A27^3+C$21*A27^2+D$21*A27+E$21</f>
-        <v>0.14134691292508222</v>
-      </c>
-      <c r="D27">
-        <f>A$22*A27^4+B$22*A27^3+C$22*A27^2+D$22*A27+E$22</f>
-        <v>1.622299602736299E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A28">
-        <v>0.1</v>
-      </c>
-      <c r="B28">
-        <f t="shared" ref="B28:B38" si="2">A$20*A28^4+B$20*A28^3+C$20*A28^2+D$20*A28+E$20</f>
-        <v>0.19262514867268199</v>
-      </c>
-      <c r="C28">
-        <f t="shared" ref="C28:C38" si="3">A$21*A28^4+B$21*A28^3+C$21*A28^2+D$21*A28+E$21</f>
-        <v>0.14593599611065727</v>
-      </c>
-      <c r="D28">
-        <f t="shared" ref="D28:D38" si="4">A$22*A28^4+B$22*A28^3+C$22*A28^2+D$22*A28+E$22</f>
-        <v>9.0061981147694356E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A29">
-        <v>0.15</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="2"/>
-        <v>0.22099013408614587</v>
-      </c>
-      <c r="C29">
-        <f t="shared" ref="C29" si="5">A$21*A29^4+B$21*A29^3+C$21*A29^2+D$21*A29+E$21</f>
-        <v>0.15187994751269807</v>
-      </c>
-      <c r="D29">
-        <f t="shared" ref="D29" si="6">A$22*A29^4+B$22*A29^3+C$22*A29^2+D$22*A29+E$22</f>
-        <v>0.11434986428587388</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A30">
-        <v>0.2</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="2"/>
-        <v>0.25081221724361547</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="3"/>
-        <v>0.15953280649103985</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="4"/>
-        <v>0.13106657169256461</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A31">
-        <v>0.3</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="2"/>
-        <v>0.31511695886641533</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="3"/>
-        <v>0.17915649329318784</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="4"/>
-        <v>0.1561847066949581</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A32">
-        <v>0.4</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="2"/>
-        <v>0.38616992155255503</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="3"/>
-        <v>0.20546178709383356</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="4"/>
-        <v>0.18962597977074175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33">
-        <v>0.5</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="2"/>
-        <v>0.46468482748916695</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="3"/>
-        <v>0.24273899981948358</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="4"/>
-        <v>0.24826094269403809</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A34">
-        <v>0.6</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="2"/>
-        <v>0.55145857303904222</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="3"/>
-        <v>0.29891402474641893</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="4"/>
-        <v>0.34162110539722546</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35">
-        <v>0.7</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="2"/>
-        <v>0.64737122874063091</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="3"/>
-        <v>0.38554833650069487</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="4"/>
-        <v>0.47189893597093802</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36">
-        <v>0.8</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="2"/>
-        <v>0.75338603930804171</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="3"/>
-        <v>0.51783899105814157</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="4"/>
-        <v>0.63394786066406683</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37">
-        <v>0.9</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="2"/>
-        <v>0.87054942363104204</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="3"/>
-        <v>0.71461862574436208</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="4"/>
-        <v>0.81528226388375635</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="2"/>
-        <v>0.99999097477505849</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="3"/>
-        <v>0.99835545923473523</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="4"/>
-        <v>0.99607748819540898</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>